<commit_message>
mid-level testing in progress 2
</commit_message>
<xml_diff>
--- a/testdata/presentation/qa_test_results_low_explicit.xlsx
+++ b/testdata/presentation/qa_test_results_low_explicit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goeastagent/products/MedicalAIMaster/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goeastagent/products/MedicalAIMaster/testdata/presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F22B6D-2B56-5346-84BF-D797EE9C9519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B1B036-B0B8-5143-AE68-0CF471B27BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="요약" sheetId="1" r:id="rId1"/>
@@ -1050,14 +1050,14 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="2" width="182" customWidth="1"/>
-    <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="67.5" customWidth="1"/>
+    <col min="2" max="2" width="147.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
     <col min="5" max="5" width="33.33203125" customWidth="1"/>
     <col min="7" max="7" width="28.83203125" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" customWidth="1"/>

</xml_diff>